<commit_message>
[expression] - [`CSV(...) => replaceColumnRegex(searchFor,replaceWith,columnNameOrIndices)`]: support search-and-replace empty and blank cells. - [`LIST(...) => replace(searchFor,replaceWith)`]: support search-and-replace empty and blank item. - [`TEXT(...) => replace(searchFor,replaceWith)`]: support search-and-replace empty and blank text.
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_expressions1.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_expressions1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\nexial\nexial-core\src\test\resources\unittesting\artifact\script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119EBFC7-DC3E-47B3-BE1A-8405FB98EC2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C7D4CD-0C81-42FD-89F5-3CCF02593936}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -61,12 +61,11 @@
     <definedName name="xml">'#system'!$AF$2:$AF$27</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2183" uniqueCount="1147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2167" uniqueCount="1158">
   <si>
     <t>target</t>
   </si>
@@ -6862,12 +6861,128 @@
   <si>
     <t>$(syspath|out|fullpath)/unitTest_expressions1.CSV.xlsx</t>
   </si>
+  <si>
+    <t>replace_empty</t>
+  </si>
+  <si>
+    <t>a|b|c|CC|d|DDDD|e|DDTABDD|f|g|CC|CC</t>
+  </si>
+  <si>
+    <t>test search-replace empty and blank chars</t>
+  </si>
+  <si>
+    <r>
+      <t>[LIST(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>a,b,c,,d,  ,e, \t ,f,g,,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>) =&gt; 
+ replace(,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>) 
+ replace( ,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>DD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>) 
+ replace(\t,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TAB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>) 
+ combine(|)
+]</t>
+    </r>
+  </si>
+  <si>
+    <t>search-replace blank chars</t>
+  </si>
+  <si>
+    <t>search-replace tab chars</t>
+  </si>
+  <si>
+    <t>[TEXT(  ) =&gt; replace( ,DD)]</t>
+  </si>
+  <si>
+    <t>DDDD</t>
+  </si>
+  <si>
+    <t>[TEXT( \t ) =&gt; replace(\t,TAB) replace( ,EE)]</t>
+  </si>
+  <si>
+    <t>EETABEE</t>
+  </si>
+  <si>
+    <t>replace_nonprintable</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7031,6 +7146,13 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -7095,7 +7217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7293,6 +7415,26 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -7321,25 +7463,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9953,12 +10091,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O136"/>
+  <dimension ref="A1:O135"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A5" sqref="A5"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
@@ -9980,12 +10118,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23.1" customHeight="1">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="65" t="s">
         <v>564</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
       <c r="E1" s="12" t="s">
         <v>565</v>
       </c>
@@ -10003,20 +10141,20 @@
       </c>
       <c r="J1" s="31"/>
       <c r="K1" s="18"/>
-      <c r="L1" s="62" t="s">
+      <c r="L1" s="67" t="s">
         <v>570</v>
       </c>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="63"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="68"/>
     </row>
     <row r="2" spans="1:15" ht="62.1" customHeight="1">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="69" t="s">
         <v>571</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
       <c r="E2" s="13"/>
       <c r="F2" s="14"/>
       <c r="G2" s="13"/>
@@ -10026,10 +10164,10 @@
       </c>
       <c r="J2" s="31"/>
       <c r="K2" s="18"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="72"/>
     </row>
     <row r="3" spans="1:15" ht="11.1" customHeight="1">
       <c r="A3" s="15"/>
@@ -12939,8 +13077,43 @@
       <c r="K115"/>
       <c r="L115"/>
     </row>
-    <row r="116" spans="1:12" ht="21" customHeight="1"/>
-    <row r="117" spans="1:12" ht="21" customHeight="1"/>
+    <row r="116" spans="1:12" ht="21" customHeight="1">
+      <c r="A116" s="74" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B116" s="75" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C116" s="77" t="s">
+        <v>5</v>
+      </c>
+      <c r="D116" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E116" s="76" t="s">
+        <v>1154</v>
+      </c>
+      <c r="F116" s="76" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" ht="21" customHeight="1">
+      <c r="B117" s="75" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C117" s="77" t="s">
+        <v>5</v>
+      </c>
+      <c r="D117" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E117" s="76" t="s">
+        <v>1156</v>
+      </c>
+      <c r="F117" s="76" t="s">
+        <v>1155</v>
+      </c>
+    </row>
     <row r="118" spans="1:12" ht="21" customHeight="1"/>
     <row r="119" spans="1:12" ht="21" customHeight="1"/>
     <row r="120" spans="1:12" ht="21" customHeight="1"/>
@@ -12959,7 +13132,6 @@
     <row r="133" ht="21" customHeight="1"/>
     <row r="134" ht="21" customHeight="1"/>
     <row r="135" ht="21" customHeight="1"/>
-    <row r="136" ht="21" customHeight="1"/>
   </sheetData>
   <sheetProtection insertRows="0" insertHyperlinks="0" deleteRows="0"/>
   <mergeCells count="4">
@@ -13001,11 +13173,11 @@
       <formula>LEFT(N3,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C110" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>target</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D110" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D110 D116:D117" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
   </dataValidations>
@@ -13019,18 +13191,18 @@
   <dimension ref="A1:O90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A5" sqref="A5"/>
-      <selection pane="bottomLeft" activeCell="B85" sqref="B85"/>
+      <selection pane="bottomLeft" activeCell="B88" sqref="B88:F88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.375" style="3" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.375" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.5" style="6" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="43.625" style="6" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="15.25" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.5" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.5" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.5" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="43.875" style="6" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="52.625" style="6" customWidth="1" collapsed="1"/>
     <col min="7" max="9" width="20" style="6" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="20" style="7" customWidth="1" collapsed="1"/>
@@ -13043,12 +13215,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23.1" customHeight="1">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="65" t="s">
         <v>564</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
       <c r="E1" s="12" t="s">
         <v>565</v>
       </c>
@@ -13066,20 +13238,20 @@
       </c>
       <c r="J1" s="31"/>
       <c r="K1" s="18"/>
-      <c r="L1" s="62" t="s">
+      <c r="L1" s="67" t="s">
         <v>570</v>
       </c>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="63"/>
-    </row>
-    <row r="2" spans="1:15" ht="93" hidden="1" customHeight="1">
-      <c r="A2" s="64" t="s">
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="68"/>
+    </row>
+    <row r="2" spans="1:15" ht="45" customHeight="1">
+      <c r="A2" s="69" t="s">
         <v>571</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
       <c r="E2" s="13"/>
       <c r="F2" s="14"/>
       <c r="G2" s="13"/>
@@ -13089,10 +13261,10 @@
       </c>
       <c r="J2" s="31"/>
       <c r="K2" s="18"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="72"/>
     </row>
     <row r="3" spans="1:15" ht="9.9499999999999993" customHeight="1">
       <c r="A3" s="15"/>
@@ -13160,9 +13332,7 @@
       <c r="A5" s="21" t="s">
         <v>659</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>659</v>
-      </c>
+      <c r="B5" s="22"/>
       <c r="C5" s="23" t="s">
         <v>5</v>
       </c>
@@ -13239,9 +13409,7 @@
       <c r="A8" s="21" t="s">
         <v>776</v>
       </c>
-      <c r="B8" s="22" t="s">
-        <v>776</v>
-      </c>
+      <c r="B8" s="22"/>
       <c r="C8" s="23" t="s">
         <v>5</v>
       </c>
@@ -13293,9 +13461,7 @@
       <c r="A10" s="21" t="s">
         <v>779</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>779</v>
-      </c>
+      <c r="B10" s="22"/>
       <c r="C10" s="23" t="s">
         <v>5</v>
       </c>
@@ -13422,9 +13588,7 @@
       <c r="A15" s="21" t="s">
         <v>622</v>
       </c>
-      <c r="B15" s="22" t="s">
-        <v>622</v>
-      </c>
+      <c r="B15" s="22"/>
       <c r="C15" s="23" t="s">
         <v>5</v>
       </c>
@@ -13476,9 +13640,7 @@
       <c r="A17" s="21" t="s">
         <v>791</v>
       </c>
-      <c r="B17" s="22" t="s">
-        <v>791</v>
-      </c>
+      <c r="B17" s="22"/>
       <c r="C17" s="23" t="s">
         <v>5</v>
       </c>
@@ -13530,9 +13692,7 @@
       <c r="A19" s="21" t="s">
         <v>795</v>
       </c>
-      <c r="B19" s="22" t="s">
-        <v>795</v>
-      </c>
+      <c r="B19" s="22"/>
       <c r="C19" s="23" t="s">
         <v>5</v>
       </c>
@@ -13584,9 +13744,7 @@
       <c r="A21" s="21" t="s">
         <v>614</v>
       </c>
-      <c r="B21" s="22" t="s">
-        <v>614</v>
-      </c>
+      <c r="B21" s="22"/>
       <c r="C21" s="23" t="s">
         <v>5</v>
       </c>
@@ -13638,9 +13796,7 @@
       <c r="A23" s="21" t="s">
         <v>801</v>
       </c>
-      <c r="B23" s="22" t="s">
-        <v>801</v>
-      </c>
+      <c r="B23" s="22"/>
       <c r="C23" s="23" t="s">
         <v>5</v>
       </c>
@@ -13692,9 +13848,7 @@
       <c r="A25" s="27" t="s">
         <v>804</v>
       </c>
-      <c r="B25" s="28" t="s">
-        <v>804</v>
-      </c>
+      <c r="B25" s="28"/>
       <c r="C25" s="23" t="s">
         <v>5</v>
       </c>
@@ -13746,9 +13900,7 @@
       <c r="A27" s="21" t="s">
         <v>601</v>
       </c>
-      <c r="B27" s="22" t="s">
-        <v>601</v>
-      </c>
+      <c r="B27" s="22"/>
       <c r="C27" s="23" t="s">
         <v>5</v>
       </c>
@@ -13800,9 +13952,7 @@
       <c r="A29" s="21" t="s">
         <v>809</v>
       </c>
-      <c r="B29" s="22" t="s">
-        <v>809</v>
-      </c>
+      <c r="B29" s="22"/>
       <c r="C29" s="23" t="s">
         <v>5</v>
       </c>
@@ -13879,9 +14029,7 @@
       <c r="A32" s="21" t="s">
         <v>815</v>
       </c>
-      <c r="B32" s="22" t="s">
-        <v>815</v>
-      </c>
+      <c r="B32" s="22"/>
       <c r="C32" s="23" t="s">
         <v>5</v>
       </c>
@@ -13933,9 +14081,7 @@
       <c r="A34" s="21" t="s">
         <v>818</v>
       </c>
-      <c r="B34" s="22" t="s">
-        <v>818</v>
-      </c>
+      <c r="B34" s="22"/>
       <c r="C34" s="23" t="s">
         <v>5</v>
       </c>
@@ -14012,9 +14158,7 @@
       <c r="A37" s="21" t="s">
         <v>822</v>
       </c>
-      <c r="B37" s="22" t="s">
-        <v>822</v>
-      </c>
+      <c r="B37" s="22"/>
       <c r="C37" s="23" t="s">
         <v>5</v>
       </c>
@@ -14066,9 +14210,7 @@
       <c r="A39" s="21" t="s">
         <v>618</v>
       </c>
-      <c r="B39" s="22" t="s">
-        <v>618</v>
-      </c>
+      <c r="B39" s="22"/>
       <c r="C39" s="23" t="s">
         <v>5</v>
       </c>
@@ -14120,9 +14262,7 @@
       <c r="A41" s="21" t="s">
         <v>826</v>
       </c>
-      <c r="B41" s="22" t="s">
-        <v>826</v>
-      </c>
+      <c r="B41" s="22"/>
       <c r="C41" s="23" t="s">
         <v>5</v>
       </c>
@@ -14174,9 +14314,7 @@
       <c r="A43" s="21" t="s">
         <v>829</v>
       </c>
-      <c r="B43" s="22" t="s">
-        <v>829</v>
-      </c>
+      <c r="B43" s="22"/>
       <c r="C43" s="23" t="s">
         <v>5</v>
       </c>
@@ -14228,9 +14366,7 @@
       <c r="A45" s="21" t="s">
         <v>725</v>
       </c>
-      <c r="B45" s="22" t="s">
-        <v>725</v>
-      </c>
+      <c r="B45" s="22"/>
       <c r="C45" s="23" t="s">
         <v>5</v>
       </c>
@@ -14282,9 +14418,7 @@
       <c r="A47" s="21" t="s">
         <v>678</v>
       </c>
-      <c r="B47" s="22" t="s">
-        <v>678</v>
-      </c>
+      <c r="B47" s="22"/>
       <c r="C47" s="23" t="s">
         <v>5</v>
       </c>
@@ -14336,9 +14470,7 @@
       <c r="A49" s="48" t="s">
         <v>594</v>
       </c>
-      <c r="B49" s="49" t="s">
-        <v>594</v>
-      </c>
+      <c r="B49" s="49"/>
       <c r="C49" s="23" t="s">
         <v>5</v>
       </c>
@@ -14390,9 +14522,7 @@
       <c r="A51" s="21" t="s">
         <v>839</v>
       </c>
-      <c r="B51" s="22" t="s">
-        <v>839</v>
-      </c>
+      <c r="B51" s="22"/>
       <c r="C51" s="23" t="s">
         <v>5</v>
       </c>
@@ -14444,9 +14574,7 @@
       <c r="A53" s="21" t="s">
         <v>598</v>
       </c>
-      <c r="B53" s="22" t="s">
-        <v>598</v>
-      </c>
+      <c r="B53" s="22"/>
       <c r="C53" s="23" t="s">
         <v>5</v>
       </c>
@@ -14498,9 +14626,7 @@
       <c r="A55" s="21" t="s">
         <v>846</v>
       </c>
-      <c r="B55" s="22" t="s">
-        <v>846</v>
-      </c>
+      <c r="B55" s="22"/>
       <c r="C55" s="23" t="s">
         <v>5</v>
       </c>
@@ -14552,9 +14678,7 @@
       <c r="A57" s="37" t="s">
         <v>656</v>
       </c>
-      <c r="B57" s="38" t="s">
-        <v>656</v>
-      </c>
+      <c r="B57" s="38"/>
       <c r="C57" s="23" t="s">
         <v>5</v>
       </c>
@@ -14606,9 +14730,7 @@
       <c r="A59" s="21" t="s">
         <v>853</v>
       </c>
-      <c r="B59" s="22" t="s">
-        <v>853</v>
-      </c>
+      <c r="B59" s="22"/>
       <c r="C59" s="23" t="s">
         <v>5</v>
       </c>
@@ -14660,9 +14782,7 @@
       <c r="A61" s="21" t="s">
         <v>857</v>
       </c>
-      <c r="B61" s="22" t="s">
-        <v>857</v>
-      </c>
+      <c r="B61" s="22"/>
       <c r="C61" s="23" t="s">
         <v>5</v>
       </c>
@@ -14714,9 +14834,7 @@
       <c r="A63" s="21" t="s">
         <v>860</v>
       </c>
-      <c r="B63" s="22" t="s">
-        <v>860</v>
-      </c>
+      <c r="B63" s="22"/>
       <c r="C63" s="23" t="s">
         <v>5</v>
       </c>
@@ -14768,9 +14886,7 @@
       <c r="A65" s="21" t="s">
         <v>641</v>
       </c>
-      <c r="B65" s="22" t="s">
-        <v>641</v>
-      </c>
+      <c r="B65" s="22"/>
       <c r="C65" s="23" t="s">
         <v>5</v>
       </c>
@@ -14847,9 +14963,7 @@
       <c r="A68" s="21" t="s">
         <v>866</v>
       </c>
-      <c r="B68" s="22" t="s">
-        <v>866</v>
-      </c>
+      <c r="B68" s="22"/>
       <c r="C68" s="23" t="s">
         <v>5</v>
       </c>
@@ -14901,9 +15015,7 @@
       <c r="A70" s="21" t="s">
         <v>868</v>
       </c>
-      <c r="B70" s="22" t="s">
-        <v>868</v>
-      </c>
+      <c r="B70" s="22"/>
       <c r="C70" s="23" t="s">
         <v>5</v>
       </c>
@@ -14955,9 +15067,7 @@
       <c r="A72" s="21" t="s">
         <v>733</v>
       </c>
-      <c r="B72" s="22" t="s">
-        <v>733</v>
-      </c>
+      <c r="B72" s="22"/>
       <c r="C72" s="23" t="s">
         <v>5</v>
       </c>
@@ -15034,9 +15144,7 @@
       <c r="A75" s="21" t="s">
         <v>873</v>
       </c>
-      <c r="B75" s="22" t="s">
-        <v>873</v>
-      </c>
+      <c r="B75" s="22"/>
       <c r="C75" s="23" t="s">
         <v>5</v>
       </c>
@@ -15113,9 +15221,7 @@
       <c r="A78" s="21" t="s">
         <v>876</v>
       </c>
-      <c r="B78" s="22" t="s">
-        <v>876</v>
-      </c>
+      <c r="B78" s="22"/>
       <c r="C78" s="23" t="s">
         <v>5</v>
       </c>
@@ -15363,13 +15469,25 @@
       <c r="N87" s="19"/>
       <c r="O87" s="18"/>
     </row>
-    <row r="88" spans="1:15" ht="23.1" customHeight="1">
-      <c r="A88" s="21"/>
-      <c r="B88" s="22"/>
-      <c r="C88" s="23"/>
-      <c r="D88" s="24"/>
-      <c r="E88" s="24"/>
-      <c r="F88" s="24"/>
+    <row r="88" spans="1:15" ht="90">
+      <c r="A88" s="21" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B88" s="22" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C88" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D88" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E88" s="73" t="s">
+        <v>1148</v>
+      </c>
+      <c r="F88" s="60" t="s">
+        <v>1150</v>
+      </c>
       <c r="G88" s="24"/>
       <c r="H88" s="24"/>
       <c r="I88" s="35"/>
@@ -15453,6 +15571,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -15460,7 +15579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A5" sqref="A5"/>
       <selection pane="bottomLeft" activeCell="A145" sqref="A145"/>
@@ -15485,12 +15604,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23.1" customHeight="1">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="65" t="s">
         <v>564</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
       <c r="E1" s="12" t="s">
         <v>565</v>
       </c>
@@ -15508,20 +15627,20 @@
       </c>
       <c r="J1" s="31"/>
       <c r="K1" s="18"/>
-      <c r="L1" s="62" t="s">
+      <c r="L1" s="67" t="s">
         <v>570</v>
       </c>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="63"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="68"/>
     </row>
     <row r="2" spans="1:15" ht="99.95" customHeight="1">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="69" t="s">
         <v>894</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
       <c r="E2" s="13"/>
       <c r="F2" s="14"/>
       <c r="G2" s="13"/>
@@ -15531,10 +15650,10 @@
       </c>
       <c r="J2" s="31"/>
       <c r="K2" s="18"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="72"/>
     </row>
     <row r="3" spans="1:15" ht="9.9499999999999993" customHeight="1">
       <c r="A3" s="15"/>
@@ -18087,7 +18206,7 @@
       <c r="N101" s="19"/>
       <c r="O101" s="18"/>
     </row>
-    <row r="102" spans="1:15" s="2" customFormat="1" ht="105">
+    <row r="102" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A102" s="21" t="s">
         <v>1058</v>
       </c>
@@ -19135,7 +19254,7 @@
     </row>
     <row r="142" spans="1:15" ht="90">
       <c r="A142" s="21"/>
-      <c r="B142" s="70" t="s">
+      <c r="B142" s="62" t="s">
         <v>1143</v>
       </c>
       <c r="C142" s="23" t="s">
@@ -19144,7 +19263,7 @@
       <c r="D142" s="24" t="s">
         <v>394</v>
       </c>
-      <c r="E142" s="68" t="s">
+      <c r="E142" s="60" t="s">
         <v>1144</v>
       </c>
       <c r="F142" s="24"/>
@@ -19169,7 +19288,7 @@
       <c r="D143" s="24" t="s">
         <v>394</v>
       </c>
-      <c r="E143" s="69" t="s">
+      <c r="E143" s="61" t="s">
         <v>1140</v>
       </c>
       <c r="F143" s="24"/>
@@ -19197,7 +19316,7 @@
       <c r="E144" s="24" t="s">
         <v>1142</v>
       </c>
-      <c r="F144" s="68" t="s">
+      <c r="F144" s="60" t="s">
         <v>1145</v>
       </c>
       <c r="G144" s="24"/>
@@ -19213,16 +19332,16 @@
     <row r="145" spans="1:15" ht="23.1" customHeight="1">
       <c r="A145" s="15"/>
       <c r="B145" s="16"/>
-      <c r="C145" s="71" t="s">
+      <c r="C145" s="63" t="s">
         <v>11</v>
       </c>
       <c r="D145" s="35" t="s">
         <v>229</v>
       </c>
-      <c r="E145" s="72" t="s">
+      <c r="E145" s="64" t="s">
         <v>1146</v>
       </c>
-      <c r="F145" s="72" t="s">
+      <c r="F145" s="64" t="s">
         <v>749</v>
       </c>
       <c r="G145" s="35"/>

</xml_diff>